<commit_message>
updated yields for dairy
</commit_message>
<xml_diff>
--- a/data/gcam_files/Gompertz_curves.xlsx
+++ b/data/gcam_files/Gompertz_curves.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM_test\gcam-sandbox\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\ManurePyrolysisIAM\data\gcam_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6508C0D2-E94C-408C-BAD4-00D6FDB7E15F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32090AE3-71A9-4DC0-A9AB-885E81EE67AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="862" yWindow="-98" windowWidth="28036" windowHeight="16395" xr2:uid="{24B5AE25-26DF-4E4B-8687-F6193DF00A4A}"/>
+    <workbookView xWindow="983" yWindow="-98" windowWidth="27915" windowHeight="16395" xr2:uid="{24B5AE25-26DF-4E4B-8687-F6193DF00A4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1281,9 +1281,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1321,7 +1321,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1427,7 +1427,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1569,7 +1569,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1580,7 +1580,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X17" sqref="X17"/>
+      <selection activeCell="D28" sqref="D28:T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1618,7 +1618,7 @@
         <v>1.381</v>
       </c>
       <c r="D3">
-        <v>0.878</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="E3">
         <v>2.589</v>
@@ -1744,7 +1744,7 @@
       </c>
       <c r="D9">
         <f t="shared" ref="D9:G23" si="3">D$3*EXP(-1*D$4*EXP(-1*D$5*$A9))</f>
-        <v>1.5969142108260281E-3</v>
+        <v>3.273856013082973E-5</v>
       </c>
       <c r="E9">
         <f t="shared" si="3"/>
@@ -1784,7 +1784,7 @@
       </c>
       <c r="D10">
         <f t="shared" si="3"/>
-        <v>1.6388418365013622E-2</v>
+        <v>3.3598124210734075E-4</v>
       </c>
       <c r="E10">
         <f t="shared" si="3"/>
@@ -1824,7 +1824,7 @@
       </c>
       <c r="D11">
         <f t="shared" si="3"/>
-        <v>7.1219037416634962E-2</v>
+        <v>1.460071382117801E-3</v>
       </c>
       <c r="E11">
         <f t="shared" si="3"/>
@@ -1864,7 +1864,7 @@
       </c>
       <c r="D12">
         <f t="shared" si="3"/>
-        <v>0.17996338277609097</v>
+        <v>3.6894543165941198E-3</v>
       </c>
       <c r="E12">
         <f t="shared" si="3"/>
@@ -1904,7 +1904,7 @@
       </c>
       <c r="D13">
         <f t="shared" si="3"/>
-        <v>0.32299814934852644</v>
+        <v>6.6218299410859627E-3</v>
       </c>
       <c r="E13">
         <f t="shared" si="3"/>
@@ -1944,7 +1944,7 @@
       </c>
       <c r="D14">
         <f t="shared" si="3"/>
-        <v>0.46716814628777442</v>
+        <v>9.5774790810705442E-3</v>
       </c>
       <c r="E14">
         <f t="shared" si="3"/>
@@ -1984,7 +1984,7 @@
       </c>
       <c r="D15">
         <f t="shared" si="3"/>
-        <v>0.58965606313420915</v>
+        <v>1.2088620884300414E-2</v>
       </c>
       <c r="E15">
         <f t="shared" si="3"/>
@@ -2024,7 +2024,7 @@
       </c>
       <c r="D16">
         <f t="shared" si="3"/>
-        <v>0.68297479155904384</v>
+        <v>1.4001761102577209E-2</v>
       </c>
       <c r="E16">
         <f t="shared" si="3"/>
@@ -2064,7 +2064,7 @@
       </c>
       <c r="D17">
         <f t="shared" si="3"/>
-        <v>0.74931336539734128</v>
+        <v>1.5361777422724534E-2</v>
       </c>
       <c r="E17">
         <f t="shared" si="3"/>
@@ -2104,7 +2104,7 @@
       </c>
       <c r="D18">
         <f t="shared" si="3"/>
-        <v>0.79444725303557251</v>
+        <v>1.6287073524647273E-2</v>
       </c>
       <c r="E18">
         <f t="shared" si="3"/>
@@ -2144,7 +2144,7 @@
       </c>
       <c r="D19">
         <f t="shared" si="3"/>
-        <v>0.82431345092826769</v>
+        <v>1.6899364597618243E-2</v>
       </c>
       <c r="E19">
         <f t="shared" si="3"/>
@@ -2184,7 +2184,7 @@
       </c>
       <c r="D20">
         <f t="shared" si="3"/>
-        <v>0.84373281669409173</v>
+        <v>1.7297483713546297E-2</v>
       </c>
       <c r="E20">
         <f t="shared" si="3"/>
@@ -2224,7 +2224,7 @@
       </c>
       <c r="D21">
         <f t="shared" si="3"/>
-        <v>0.85622032266976023</v>
+        <v>1.7553491808719457E-2</v>
       </c>
       <c r="E21">
         <f t="shared" si="3"/>
@@ -2264,7 +2264,7 @@
       </c>
       <c r="D22">
         <f t="shared" si="3"/>
-        <v>0.86419432932199669</v>
+        <v>1.7716968027102434E-2</v>
       </c>
       <c r="E22">
         <f t="shared" si="3"/>
@@ -2304,7 +2304,7 @@
       </c>
       <c r="D23">
         <f t="shared" si="3"/>
-        <v>0.86926375403176959</v>
+        <v>1.7820897007485025E-2</v>
       </c>
       <c r="E23">
         <f t="shared" si="3"/>
@@ -2344,7 +2344,7 @@
       </c>
       <c r="D24">
         <f t="shared" si="2"/>
-        <v>0.87247763472088735</v>
+        <v>1.7886785222068304E-2</v>
       </c>
       <c r="E24">
         <f t="shared" si="2"/>
@@ -2384,7 +2384,7 @@
       </c>
       <c r="D25">
         <f t="shared" si="2"/>
-        <v>0.87451156749982806</v>
+        <v>1.7928483160588728E-2</v>
       </c>
       <c r="E25">
         <f t="shared" si="2"/>

</xml_diff>

<commit_message>
ensure no duplicates in mask list
</commit_message>
<xml_diff>
--- a/data/gcam_files/Gompertz_curves.xlsx
+++ b/data/gcam_files/Gompertz_curves.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\ManurePyrolysisIAM\data\gcam_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\natha\PycharmProjects\IAM_test\drawing_figures\data\gcam_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32090AE3-71A9-4DC0-A9AB-885E81EE67AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BB66950-5FF1-42E6-A0FE-B01A1EDFFD47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="983" yWindow="-98" windowWidth="27915" windowHeight="16395" xr2:uid="{24B5AE25-26DF-4E4B-8687-F6193DF00A4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{24B5AE25-26DF-4E4B-8687-F6193DF00A4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>b</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Poultry</t>
   </si>
   <si>
-    <t>Dairy</t>
-  </si>
-  <si>
     <t>Beef</t>
   </si>
   <si>
@@ -75,6 +72,12 @@
   </si>
   <si>
     <t>Gompertz</t>
+  </si>
+  <si>
+    <t>Dairy (pyrolysis)</t>
+  </si>
+  <si>
+    <t>Dairy (pyrolysis-nofert)</t>
   </si>
 </sst>
 </file>
@@ -164,7 +167,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$I$7</c:f>
+              <c:f>Sheet1!$J$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -187,7 +190,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$H$8:$H$25</c:f>
+              <c:f>Sheet1!$I$8:$I$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -250,7 +253,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$I$8:$I$25</c:f>
+              <c:f>Sheet1!$J$8:$J$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -323,7 +326,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$J$7</c:f>
+              <c:f>Sheet1!$K$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -346,7 +349,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$H$8:$H$25</c:f>
+              <c:f>Sheet1!$I$8:$I$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -409,7 +412,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$J$8:$J$25</c:f>
+              <c:f>Sheet1!$K$8:$K$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="18"/>
@@ -1243,13 +1246,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
@@ -1577,40 +1580,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B34577B2-BEF4-400B-8752-038474EAFFFD}">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28:T28"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>5</v>
       </c>
@@ -1618,19 +1625,22 @@
         <v>1.381</v>
       </c>
       <c r="D3">
+        <v>0.878</v>
+      </c>
+      <c r="E3">
         <v>1.7999999999999999E-2</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>2.589</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.30399999999999999</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>3.101</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -1649,8 +1659,11 @@
       <c r="G4">
         <v>10</v>
       </c>
+      <c r="H4">
+        <v>10</v>
+      </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -1659,23 +1672,27 @@
         <v>9.2103403719761834E-2</v>
       </c>
       <c r="D5">
-        <f t="shared" ref="D5:F5" si="0">LN(D4)/$A$13</f>
+        <f t="shared" ref="D5" si="0">LN(D4)/$A$13</f>
         <v>9.2103403719761834E-2</v>
       </c>
       <c r="E5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="E5:G5" si="1">LN(E4)/$A$13</f>
         <v>9.2103403719761834E-2</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9.2103403719761834E-2</v>
       </c>
       <c r="G5">
-        <f>LN(G4)/$A$13</f>
+        <f t="shared" si="1"/>
         <v>9.2103403719761834E-2</v>
       </c>
+      <c r="H5">
+        <f>LN(H4)/$A$13</f>
+        <v>9.2103403719761834E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1685,17 +1702,17 @@
       <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" t="s">
         <v>12</v>
       </c>
-      <c r="I7" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7">
+      <c r="K7">
         <v>2070</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>0</v>
       </c>
@@ -1719,694 +1736,765 @@
         <v>0</v>
       </c>
       <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
         <f>B8</f>
         <v>2015</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <f>C8/$C$3*100</f>
         <v>0</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9">
-        <f t="shared" ref="B9:B25" si="1">2015+A9</f>
+        <f t="shared" ref="B9:B25" si="2">2015+A9</f>
         <v>2020</v>
       </c>
       <c r="C9">
-        <f t="shared" ref="C9:G25" si="2">C$3*EXP(-1*C$4*EXP(-1*C$5*$A9))</f>
+        <f t="shared" ref="C9:H25" si="3">C$3*EXP(-1*C$4*EXP(-1*C$5*$A9))</f>
         <v>2.5117750855931033E-3</v>
       </c>
       <c r="D9">
-        <f t="shared" ref="D9:G23" si="3">D$3*EXP(-1*D$4*EXP(-1*D$5*$A9))</f>
+        <f t="shared" ref="D9:H23" si="4">D$3*EXP(-1*D$4*EXP(-1*D$5*$A9))</f>
+        <v>1.5969142108260281E-3</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="4"/>
         <v>3.273856013082973E-5</v>
       </c>
-      <c r="E9">
-        <f t="shared" si="3"/>
+      <c r="F9">
+        <f t="shared" si="4"/>
         <v>4.70889623215101E-3</v>
       </c>
-      <c r="F9">
-        <f t="shared" si="3"/>
+      <c r="G9">
+        <f t="shared" si="4"/>
         <v>5.5291790443179106E-4</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="3"/>
+      <c r="H9">
+        <f t="shared" si="4"/>
         <v>5.6401263869834996E-3</v>
       </c>
-      <c r="H9">
-        <f t="shared" ref="H9:H25" si="4">B9</f>
+      <c r="I9">
+        <f t="shared" ref="I9:I25" si="5">B9</f>
         <v>2020</v>
       </c>
-      <c r="I9">
-        <f t="shared" ref="I9:I25" si="5">C9/$C$3*100</f>
+      <c r="J9">
+        <f t="shared" ref="J9:J25" si="6">C9/$C$3*100</f>
         <v>0.18188088961572074</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2025</v>
       </c>
       <c r="C10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.5777227519457643E-2</v>
       </c>
       <c r="D10">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>1.6388418365013622E-2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="4"/>
         <v>3.3598124210734075E-4</v>
       </c>
-      <c r="E10">
-        <f t="shared" si="3"/>
+      <c r="F10">
+        <f t="shared" si="4"/>
         <v>4.8325301989772508E-2</v>
       </c>
-      <c r="F10">
-        <f t="shared" si="3"/>
+      <c r="G10">
+        <f t="shared" si="4"/>
         <v>5.674349866701755E-3</v>
       </c>
-      <c r="G10">
-        <f t="shared" si="3"/>
+      <c r="H10">
+        <f t="shared" si="4"/>
         <v>5.7882101765270207E-2</v>
-      </c>
-      <c r="H10">
-        <f t="shared" si="4"/>
-        <v>2025</v>
       </c>
       <c r="I10">
         <f t="shared" si="5"/>
+        <v>2025</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="6"/>
         <v>1.866562456151893</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>15</v>
       </c>
       <c r="B11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2030</v>
       </c>
       <c r="C11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.11201992103914907</v>
       </c>
       <c r="D11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>7.1219037416634962E-2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="4"/>
         <v>1.460071382117801E-3</v>
       </c>
-      <c r="E11">
-        <f t="shared" si="3"/>
+      <c r="F11">
+        <f t="shared" si="4"/>
         <v>0.21000693379461038</v>
       </c>
-      <c r="F11">
-        <f t="shared" si="3"/>
+      <c r="G11">
+        <f t="shared" si="4"/>
         <v>2.4658983342433972E-2</v>
       </c>
-      <c r="G11">
-        <f t="shared" si="3"/>
+      <c r="H11">
+        <f t="shared" si="4"/>
         <v>0.25153785310818338</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="4"/>
-        <v>2030</v>
       </c>
       <c r="I11">
         <f t="shared" si="5"/>
+        <v>2030</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="6"/>
         <v>8.1115076784322291</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>20</v>
       </c>
       <c r="B12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2035</v>
       </c>
       <c r="C12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.28306313395647115</v>
       </c>
       <c r="D12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0.17996338277609097</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="4"/>
         <v>3.6894543165941198E-3</v>
       </c>
-      <c r="E12">
-        <f t="shared" si="3"/>
+      <c r="F12">
+        <f t="shared" si="4"/>
         <v>0.53066651253678765</v>
       </c>
-      <c r="F12">
-        <f t="shared" si="3"/>
+      <c r="G12">
+        <f t="shared" si="4"/>
         <v>6.2310784013589589E-2</v>
       </c>
-      <c r="G12">
-        <f t="shared" si="3"/>
+      <c r="H12">
+        <f t="shared" si="4"/>
         <v>0.6356109908754648</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="4"/>
-        <v>2035</v>
       </c>
       <c r="I12">
         <f t="shared" si="5"/>
+        <v>2035</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="6"/>
         <v>20.496968425522894</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>25</v>
       </c>
       <c r="B13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2040</v>
       </c>
       <c r="C13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.50804150825776195</v>
       </c>
       <c r="D13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0.32299814934852644</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="4"/>
         <v>6.6218299410859627E-3</v>
       </c>
-      <c r="E13">
-        <f t="shared" si="3"/>
+      <c r="F13">
+        <f t="shared" si="4"/>
         <v>0.95243987319286438</v>
       </c>
-      <c r="F13">
-        <f t="shared" si="3"/>
+      <c r="G13">
+        <f t="shared" si="4"/>
         <v>0.11183535011611849</v>
       </c>
-      <c r="G13">
-        <f t="shared" si="3"/>
+      <c r="H13">
+        <f t="shared" si="4"/>
         <v>1.1407941470726428</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="4"/>
-        <v>2040</v>
       </c>
       <c r="I13">
         <f t="shared" si="5"/>
+        <v>2040</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="6"/>
         <v>36.787944117144242</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>30</v>
       </c>
       <c r="B14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2045</v>
       </c>
       <c r="C14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.73480547838657906</v>
       </c>
       <c r="D14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0.46716814628777442</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="4"/>
         <v>9.5774790810705442E-3</v>
       </c>
-      <c r="E14">
-        <f t="shared" si="3"/>
+      <c r="F14">
+        <f t="shared" si="4"/>
         <v>1.3775607411606468</v>
       </c>
-      <c r="F14">
-        <f t="shared" si="3"/>
+      <c r="G14">
+        <f t="shared" si="4"/>
         <v>0.16175298003585811</v>
       </c>
-      <c r="G14">
-        <f t="shared" si="3"/>
+      <c r="H14">
+        <f t="shared" si="4"/>
         <v>1.6499868127999868</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="4"/>
-        <v>2045</v>
       </c>
       <c r="I14">
         <f t="shared" si="5"/>
+        <v>2045</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="6"/>
         <v>53.208217117058588</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>35</v>
       </c>
       <c r="B15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2050</v>
       </c>
       <c r="C15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.92746585784549296</v>
       </c>
       <c r="D15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0.58965606313420915</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="4"/>
         <v>1.2088620884300414E-2</v>
       </c>
-      <c r="E15">
-        <f t="shared" si="3"/>
+      <c r="F15">
+        <f t="shared" si="4"/>
         <v>1.7387466371918763</v>
       </c>
-      <c r="F15">
-        <f t="shared" si="3"/>
+      <c r="G15">
+        <f t="shared" si="4"/>
         <v>0.20416337493485145</v>
       </c>
-      <c r="G15">
-        <f t="shared" si="3"/>
+      <c r="H15">
+        <f t="shared" si="4"/>
         <v>2.0826007423453103</v>
-      </c>
-      <c r="H15">
-        <f t="shared" si="4"/>
-        <v>2050</v>
       </c>
       <c r="I15">
         <f t="shared" si="5"/>
+        <v>2050</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="6"/>
         <v>67.159004912780091</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>40</v>
       </c>
       <c r="B16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2055</v>
       </c>
       <c r="C16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.074246226814396</v>
       </c>
       <c r="D16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0.68297479155904384</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="4"/>
         <v>1.4001761102577209E-2</v>
       </c>
-      <c r="E16">
-        <f t="shared" si="3"/>
+      <c r="F16">
+        <f t="shared" si="4"/>
         <v>2.0139199719206884</v>
       </c>
-      <c r="F16">
-        <f t="shared" si="3"/>
+      <c r="G16">
+        <f t="shared" si="4"/>
         <v>0.23647418751019286</v>
       </c>
-      <c r="G16">
-        <f t="shared" si="3"/>
+      <c r="H16">
+        <f t="shared" si="4"/>
         <v>2.4121922877273292</v>
-      </c>
-      <c r="H16">
-        <f t="shared" si="4"/>
-        <v>2055</v>
       </c>
       <c r="I16">
         <f t="shared" si="5"/>
+        <v>2055</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="6"/>
         <v>77.787561680984496</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>45</v>
       </c>
       <c r="B17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2060</v>
       </c>
       <c r="C17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1785897011545881</v>
       </c>
       <c r="D17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0.74931336539734128</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="4"/>
         <v>1.5361777422724534E-2</v>
       </c>
-      <c r="E17">
-        <f t="shared" si="3"/>
+      <c r="F17">
+        <f t="shared" si="4"/>
         <v>2.2095356526352123</v>
       </c>
-      <c r="F17">
-        <f t="shared" si="3"/>
+      <c r="G17">
+        <f t="shared" si="4"/>
         <v>0.2594433520282366</v>
       </c>
-      <c r="G17">
-        <f t="shared" si="3"/>
+      <c r="H17">
+        <f t="shared" si="4"/>
         <v>2.6464928771038214</v>
-      </c>
-      <c r="H17">
-        <f t="shared" si="4"/>
-        <v>2060</v>
       </c>
       <c r="I17">
         <f t="shared" si="5"/>
+        <v>2060</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="6"/>
         <v>85.343207904025192</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>50</v>
       </c>
       <c r="B18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2065</v>
       </c>
       <c r="C18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2495804743076602</v>
       </c>
       <c r="D18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0.79444725303557251</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="4"/>
         <v>1.6287073524647273E-2</v>
       </c>
-      <c r="E18">
-        <f t="shared" si="3"/>
+      <c r="F18">
+        <f t="shared" si="4"/>
         <v>2.3426240752950993</v>
       </c>
-      <c r="F18">
-        <f t="shared" si="3"/>
+      <c r="G18">
+        <f t="shared" si="4"/>
         <v>0.2750705750829317</v>
       </c>
-      <c r="G18">
-        <f t="shared" si="3"/>
+      <c r="H18">
+        <f t="shared" si="4"/>
         <v>2.8059008333295106</v>
-      </c>
-      <c r="H18">
-        <f t="shared" si="4"/>
-        <v>2065</v>
       </c>
       <c r="I18">
         <f t="shared" si="5"/>
+        <v>2065</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="6"/>
         <v>90.483741803595947</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>55</v>
       </c>
       <c r="B19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2070</v>
       </c>
       <c r="C19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.2965568060728219</v>
       </c>
       <c r="D19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0.82431345092826769</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="4"/>
         <v>1.6899364597618243E-2</v>
       </c>
-      <c r="E19">
-        <f t="shared" si="3"/>
+      <c r="F19">
+        <f t="shared" si="4"/>
         <v>2.4306919412907573</v>
       </c>
-      <c r="F19">
-        <f t="shared" si="3"/>
+      <c r="G19">
+        <f t="shared" si="4"/>
         <v>0.28541149098199697</v>
       </c>
-      <c r="G19">
-        <f t="shared" si="3"/>
+      <c r="H19">
+        <f t="shared" si="4"/>
         <v>2.9113849787341208</v>
-      </c>
-      <c r="H19">
-        <f t="shared" si="4"/>
-        <v>2070</v>
       </c>
       <c r="I19">
         <f t="shared" si="5"/>
+        <v>2070</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="6"/>
         <v>93.885358875656905</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>60</v>
       </c>
       <c r="B20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2075</v>
       </c>
       <c r="C20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3271013893559689</v>
       </c>
       <c r="D20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0.84373281669409173</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="4"/>
         <v>1.7297483713546297E-2</v>
       </c>
-      <c r="E20">
-        <f t="shared" si="3"/>
+      <c r="F20">
+        <f t="shared" si="4"/>
         <v>2.4879547407984091</v>
       </c>
-      <c r="F20">
-        <f t="shared" si="3"/>
+      <c r="G20">
+        <f t="shared" si="4"/>
         <v>0.29213528049544857</v>
       </c>
-      <c r="G20">
-        <f t="shared" si="3"/>
+      <c r="H20">
+        <f t="shared" si="4"/>
         <v>2.9799720553170594</v>
-      </c>
-      <c r="H20">
-        <f t="shared" si="4"/>
-        <v>2075</v>
       </c>
       <c r="I20">
         <f t="shared" si="5"/>
+        <v>2075</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="6"/>
         <v>96.097131741923889</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>65</v>
       </c>
       <c r="B21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2080</v>
       </c>
       <c r="C21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3467428993245318</v>
       </c>
       <c r="D21">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0.85622032266976023</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="4"/>
         <v>1.7553491808719457E-2</v>
       </c>
-      <c r="E21">
-        <f t="shared" si="3"/>
+      <c r="F21">
+        <f t="shared" si="4"/>
         <v>2.524777238487482</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="3"/>
+      <c r="G21">
+        <f t="shared" si="4"/>
         <v>0.29645897276948419</v>
       </c>
-      <c r="G21">
-        <f t="shared" si="3"/>
+      <c r="H21">
+        <f t="shared" si="4"/>
         <v>3.0240765610466136</v>
-      </c>
-      <c r="H21">
-        <f t="shared" si="4"/>
-        <v>2080</v>
       </c>
       <c r="I21">
         <f t="shared" si="5"/>
+        <v>2080</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="6"/>
         <v>97.519398937330322</v>
       </c>
-      <c r="J21">
+      <c r="K21">
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>70</v>
       </c>
       <c r="B22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2085</v>
       </c>
       <c r="C22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3592851580793592</v>
       </c>
       <c r="D22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0.86419432932199669</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="4"/>
         <v>1.7716968027102434E-2</v>
       </c>
-      <c r="E22">
-        <f t="shared" si="3"/>
+      <c r="F22">
+        <f t="shared" si="4"/>
         <v>2.5482905678982339</v>
       </c>
-      <c r="F22">
-        <f t="shared" si="3"/>
+      <c r="G22">
+        <f t="shared" si="4"/>
         <v>0.29921990445773006</v>
       </c>
-      <c r="G22">
-        <f t="shared" si="3"/>
+      <c r="H22">
+        <f t="shared" si="4"/>
         <v>3.0522398806691475</v>
-      </c>
-      <c r="H22">
-        <f t="shared" si="4"/>
-        <v>2085</v>
       </c>
       <c r="I22">
         <f t="shared" si="5"/>
+        <v>2085</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="6"/>
         <v>98.427600150569091</v>
       </c>
-      <c r="J22">
+      <c r="K22">
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>75</v>
       </c>
       <c r="B23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2090</v>
       </c>
       <c r="C23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.367258820407601</v>
       </c>
       <c r="D23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
+        <v>0.86926375403176959</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="4"/>
         <v>1.7820897007485025E-2</v>
       </c>
-      <c r="E23">
-        <f t="shared" si="3"/>
+      <c r="F23">
+        <f t="shared" si="4"/>
         <v>2.5632390195765962</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="3"/>
+      <c r="G23">
+        <f t="shared" si="4"/>
         <v>0.30097514945974707</v>
       </c>
-      <c r="G23">
-        <f t="shared" si="3"/>
+      <c r="H23">
+        <f t="shared" si="4"/>
         <v>3.0701445344561704</v>
-      </c>
-      <c r="H23">
-        <f t="shared" si="4"/>
-        <v>2090</v>
       </c>
       <c r="I23">
         <f t="shared" si="5"/>
+        <v>2090</v>
+      </c>
+      <c r="J23">
+        <f t="shared" si="6"/>
         <v>99.004983374916804</v>
       </c>
-      <c r="J23">
+      <c r="K23">
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>80</v>
       </c>
       <c r="B24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2095</v>
       </c>
       <c r="C24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.372313910648685</v>
       </c>
       <c r="D24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>0.87247763472088735</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="3"/>
         <v>1.7886785222068304E-2</v>
       </c>
-      <c r="E24">
-        <f t="shared" si="2"/>
+      <c r="F24">
+        <f t="shared" si="3"/>
         <v>2.5727159411074911</v>
       </c>
-      <c r="F24">
-        <f t="shared" si="2"/>
+      <c r="G24">
+        <f t="shared" si="3"/>
         <v>0.30208792819493135</v>
       </c>
-      <c r="G24">
-        <f t="shared" si="2"/>
+      <c r="H24">
+        <f t="shared" si="3"/>
         <v>3.0814956096463231</v>
-      </c>
-      <c r="H24">
-        <f t="shared" si="4"/>
-        <v>2095</v>
       </c>
       <c r="I24">
         <f t="shared" si="5"/>
+        <v>2095</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="6"/>
         <v>99.371029011490592</v>
       </c>
-      <c r="J24">
+      <c r="K24">
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>85</v>
       </c>
       <c r="B25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2100</v>
       </c>
       <c r="C25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3755130691540576</v>
       </c>
       <c r="D25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
+        <v>0.87451156749982806</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="3"/>
         <v>1.7928483160588728E-2</v>
       </c>
-      <c r="E25">
-        <f t="shared" si="2"/>
+      <c r="F25">
+        <f t="shared" si="3"/>
         <v>2.5787134945980124</v>
       </c>
-      <c r="F25">
-        <f t="shared" si="2"/>
+      <c r="G25">
+        <f t="shared" si="3"/>
         <v>0.30279216004549853</v>
       </c>
-      <c r="G25">
-        <f t="shared" si="2"/>
+      <c r="H25">
+        <f t="shared" si="3"/>
         <v>3.0886792378325363</v>
-      </c>
-      <c r="H25">
-        <f t="shared" si="4"/>
-        <v>2100</v>
       </c>
       <c r="I25">
         <f t="shared" si="5"/>
+        <v>2100</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="6"/>
         <v>99.602684225492936</v>
       </c>
-      <c r="J25">
+      <c r="K25">
         <v>100</v>
       </c>
     </row>

</xml_diff>